<commit_message>
suggested changes, original files, EDA, Readme.txt
</commit_message>
<xml_diff>
--- a/source_files/Region_LA_buildings.xlsx
+++ b/source_files/Region_LA_buildings.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Fintech Sandpit\ESG-entity-generator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Fintech Sandpit\ESG-entity-generator\source_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09F484E8-8AB2-46DC-8390-BBC8B6AD40A7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{031833FD-3EFE-4799-A50B-8CF7195FB298}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{86755C6B-ACE2-46DF-9925-663C115C7798}"/>
   </bookViews>
@@ -2639,7 +2639,8 @@
   <dimension ref="A1:AH369"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" activeCellId="5" sqref="A1:XFD1 A2:XFD2 A3:XFD3 A1:A1048576 B1:B1048576 C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>